<commit_message>
add data for excel
</commit_message>
<xml_diff>
--- a/excelTemplate/excelTemplate.xlsx
+++ b/excelTemplate/excelTemplate.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\myresource\githubAllCode\handle_office_server\handle_office_service\excelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="橱柜报价清单" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,10 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
-    <t>定制橱柜结算报价清单</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>订单号</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -224,6 +220,10 @@
   </si>
   <si>
     <t>总计</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>定制橱柜结算报价清单</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -587,6 +587,91 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -596,41 +681,26 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -640,17 +710,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -667,89 +737,19 @@
     <xf numFmtId="177" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1108,230 +1108,233 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="17" max="17" width="13.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="65" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="13.5" customHeight="1">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="14.25">
+      <c r="A3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="66"/>
-      <c r="R1" s="1"/>
-    </row>
-    <row r="2" spans="1:18" ht="13.5" customHeight="1">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="14.25">
-      <c r="A3" s="55" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="55" t="s">
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="55" t="s">
+      <c r="N3" s="33"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="14.25">
+      <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="58"/>
-      <c r="O3" s="56"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="14.25">
-      <c r="A4" s="55" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="55" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="55" t="s">
+      <c r="N4" s="33"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="14.25">
+      <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="58"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" ht="14.25">
-      <c r="A5" s="55" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="56"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="55" t="s">
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="56"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="55" t="s">
+      <c r="N5" s="33"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="18.75">
+      <c r="A6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="N5" s="58"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="56"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="6" spans="1:18" ht="18.75">
-      <c r="A6" s="22" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
+      <c r="Q6" s="46"/>
+      <c r="R6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" ht="14.25">
+      <c r="A7" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="14.25">
-      <c r="A7" s="50" t="s">
+      <c r="B7" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="39" t="s">
+      <c r="C7" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="D7" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="39" t="s">
+      <c r="E7" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="53" t="s">
+      <c r="I7" s="51"/>
+      <c r="J7" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="45" t="s">
+      <c r="K7" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K7" s="45" t="s">
+      <c r="L7" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="L7" s="45" t="s">
+      <c r="M7" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="36" t="s">
+      <c r="N7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="36" t="s">
+      <c r="O7" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="O7" s="36" t="s">
+      <c r="P7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="P7" s="36" t="s">
+      <c r="Q7" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="Q7" s="39" t="s">
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" ht="14.25">
+      <c r="A8" s="47"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" ht="14.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="I8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
+      <c r="J8" s="52"/>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
       <c r="P8" s="37"/>
-      <c r="Q8" s="39"/>
+      <c r="Q8" s="38"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="14.25">
@@ -1375,121 +1378,121 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="14.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="42"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="18.75">
+      <c r="A12" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="33"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="1"/>
-    </row>
-    <row r="12" spans="1:18" ht="18.75">
-      <c r="A12" s="22" t="s">
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="45"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="14.25">
+      <c r="A13" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="1"/>
-    </row>
-    <row r="13" spans="1:18" ht="14.25">
-      <c r="A13" s="46" t="s">
+      <c r="B13" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="48" t="s">
+      <c r="D13" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="40" t="s">
+      <c r="I13" s="61"/>
+      <c r="J13" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="N13" s="36" t="s">
+      <c r="O13" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="O13" s="36" t="s">
+      <c r="P13" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="36" t="s">
+      <c r="Q13" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="Q13" s="38" t="s">
-        <v>38</v>
-      </c>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="14.25">
-      <c r="A14" s="46"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="46"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="57"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
       <c r="O14" s="37"/>
       <c r="P14" s="37"/>
-      <c r="Q14" s="38"/>
+      <c r="Q14" s="53"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" ht="14.25">
@@ -1500,8 +1503,8 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="35"/>
+      <c r="H15" s="54"/>
+      <c r="I15" s="55"/>
       <c r="J15" s="19"/>
       <c r="K15" s="20"/>
       <c r="L15" s="21"/>
@@ -1520,8 +1523,8 @@
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="35"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="55"/>
       <c r="J16" s="11"/>
       <c r="K16" s="20"/>
       <c r="L16" s="21"/>
@@ -1533,121 +1536,121 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" ht="14.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" ht="18.75">
+      <c r="A18" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="1"/>
-    </row>
-    <row r="18" spans="1:18" ht="18.75">
-      <c r="A18" s="22" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" ht="14.25">
+      <c r="A19" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="61"/>
+      <c r="J19" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="M19" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="1"/>
-    </row>
-    <row r="19" spans="1:18" ht="14.25">
-      <c r="A19" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I19" s="41"/>
-      <c r="J19" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="36" t="s">
+      <c r="N19" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="N19" s="36" t="s">
+      <c r="O19" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="O19" s="36" t="s">
+      <c r="P19" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="P19" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q19" s="38" t="s">
-        <v>38</v>
+      <c r="Q19" s="53" t="s">
+        <v>37</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="14.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="46"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="56"/>
       <c r="E20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
       <c r="M20" s="37"/>
       <c r="N20" s="37"/>
       <c r="O20" s="37"/>
       <c r="P20" s="37"/>
-      <c r="Q20" s="38"/>
+      <c r="Q20" s="53"/>
       <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:18" ht="14.25">
@@ -1658,8 +1661,8 @@
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="35"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="55"/>
       <c r="J21" s="19"/>
       <c r="K21" s="20"/>
       <c r="L21" s="21"/>
@@ -1678,8 +1681,8 @@
       <c r="E22" s="18"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="35"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="55"/>
       <c r="J22" s="19"/>
       <c r="K22" s="20"/>
       <c r="L22" s="21"/>
@@ -1691,119 +1694,119 @@
       <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:18" ht="14.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="40"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="43"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" ht="18.75">
+      <c r="A24" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="25"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="1"/>
-    </row>
-    <row r="24" spans="1:18" ht="18.75">
-      <c r="A24" s="22" t="s">
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="24"/>
-      <c r="R24" s="1"/>
-    </row>
-    <row r="25" spans="1:18">
-      <c r="A25" s="46" t="s">
+      <c r="B25" s="57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="61"/>
+      <c r="J25" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="K25" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="L25" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="N25" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="G25" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="H25" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="K25" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="L25" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="N25" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="O25" s="36" t="s">
-        <v>48</v>
-      </c>
       <c r="P25" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q25" s="38" t="s">
-        <v>38</v>
+        <v>22</v>
+      </c>
+      <c r="Q25" s="53" t="s">
+        <v>37</v>
       </c>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" ht="14.25">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="44"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
+    <row r="26" spans="1:18">
+      <c r="A26" s="56"/>
+      <c r="B26" s="57"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
       <c r="M26" s="37"/>
       <c r="N26" s="37"/>
       <c r="O26" s="37"/>
       <c r="P26" s="37"/>
-      <c r="Q26" s="38"/>
+      <c r="Q26" s="53"/>
       <c r="R26" s="1"/>
     </row>
     <row r="27" spans="1:18" ht="14.25">
@@ -1814,8 +1817,8 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="35"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="55"/>
       <c r="J27" s="19"/>
       <c r="K27" s="20"/>
       <c r="L27" s="21"/>
@@ -1834,8 +1837,8 @@
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="35"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="55"/>
       <c r="J28" s="19"/>
       <c r="K28" s="20"/>
       <c r="L28" s="21"/>
@@ -1847,69 +1850,69 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" spans="1:18" ht="14.25">
-      <c r="A29" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="26"/>
+      <c r="A29" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="43"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18">
-      <c r="A30" s="27" t="s">
+    <row r="30" spans="1:18" ht="14.25">
+      <c r="A30" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="65"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="66"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="66"/>
+      <c r="M30" s="66"/>
+      <c r="N30" s="66"/>
+      <c r="O30" s="66"/>
+      <c r="P30" s="66"/>
+      <c r="Q30" s="66"/>
+      <c r="R30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" ht="14.25">
+      <c r="A31" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
-      <c r="O30" s="28"/>
-      <c r="P30" s="28"/>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="1"/>
-    </row>
-    <row r="31" spans="1:18">
-      <c r="A31" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="30"/>
-      <c r="K31" s="30"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30"/>
-      <c r="O31" s="30"/>
-      <c r="P31" s="30"/>
-      <c r="Q31" s="30"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
       <c r="R31" s="1"/>
     </row>
     <row r="32" spans="1:18">
@@ -1995,68 +1998,31 @@
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="D1:Q2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="M5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="P11:Q11"/>
-    <mergeCell ref="A6:Q6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="A12:Q12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="H13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A17:O17"/>
-    <mergeCell ref="P17:Q17"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="A24:Q24"/>
+    <mergeCell ref="P29:Q29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:Q30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:Q31"/>
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="H25:I26"/>
+    <mergeCell ref="J25:J26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:L26"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="P23:Q23"/>
     <mergeCell ref="O19:O20"/>
@@ -2070,31 +2036,68 @@
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="N19:N20"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="H25:I26"/>
-    <mergeCell ref="J25:J26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:L26"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="A24:Q24"/>
-    <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:Q30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:Q31"/>
-    <mergeCell ref="A29:O29"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A17:O17"/>
+    <mergeCell ref="P17:Q17"/>
+    <mergeCell ref="A18:Q18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="A12:Q12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="H13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="Q13:Q14"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="P11:Q11"/>
+    <mergeCell ref="A6:Q6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="D1:Q2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:Q3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>